<commit_message>
Update sources for forest management potential and costs, and add deforestation policy.
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\AOCoLUPpUA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E0273B-F952-4466-8CA6-022ECA3D5CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,18 @@
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,9 +89,6 @@
     <t>annual maintenance cost ($ / acre)</t>
   </si>
   <si>
-    <t>Avoid deforestion, peatland restoration, and forest restoration policies</t>
-  </si>
-  <si>
     <t>are not used in the U.S. version of the model.</t>
   </si>
   <si>
@@ -202,12 +216,15 @@
   </si>
   <si>
     <t>timber harvesting need to be managed.</t>
+  </si>
+  <si>
+    <t>Peatland restoration and forest restoration policies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,32 +371,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="5"/>
-    <cellStyle name="Table title" xfId="6"/>
+    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -389,6 +409,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Conversion Factors"/>
       <sheetName val="About"/>
       <sheetName val="CO2 Aff &amp; Ref"/>
       <sheetName val="VFC-PIIiCRfAaREY"/>
@@ -408,10 +429,15 @@
       <sheetName val="VFC-LVpMCAbAD"/>
       <sheetName val="County Data"/>
       <sheetName val="Forest Mgmt Costs"/>
-      <sheetName val="Conversion Factors"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="A4">
+            <v>3.6666666666666665</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
@@ -430,13 +456,7 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
-        <row r="4">
-          <cell r="A4">
-            <v>3.6666666666666665</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="19"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -485,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,9 +538,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,6 +590,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -728,10 +782,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -745,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,17 +811,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -775,12 +831,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -790,7 +846,7 @@
     </row>
     <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -821,22 +877,22 @@
     <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,27 +900,27 @@
         <v>1.278</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -876,25 +932,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <f>50+1614</f>
@@ -907,7 +963,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <f>972+4013</f>
@@ -920,7 +976,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <f>3955+13315</f>
@@ -933,7 +989,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <f>2879+2953</f>
@@ -946,7 +1002,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <f>6236+2826</f>
@@ -959,7 +1015,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <f>2156+2707</f>
@@ -972,7 +1028,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <f>2918+12457</f>
@@ -985,7 +1041,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <f>15095+29814</f>
@@ -998,7 +1054,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <f>10315+29977</f>
@@ -1011,7 +1067,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1019,31 +1075,31 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <f>39/10</f>
@@ -1056,7 +1112,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>95.55</v>
@@ -1065,27 +1121,27 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>44.67</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <f>C23*(B18/B23)</f>
         <v>13.041950354609931</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>58.48</v>
@@ -1096,12 +1152,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <f>21.5/10</f>
@@ -1114,7 +1170,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>65.11</v>
@@ -1123,12 +1179,12 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>50.76</v>
@@ -1139,7 +1195,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>58.48</v>
@@ -1150,12 +1206,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <f>21.61/10</f>
@@ -1168,7 +1224,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>65.11</v>
@@ -1177,12 +1233,12 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>50.76</v>
@@ -1193,7 +1249,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>58.48</v>
@@ -1204,12 +1260,12 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <f>24.49/10</f>
@@ -1222,9 +1278,9 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="10">
+        <v>38</v>
+      </c>
+      <c r="B32" s="8">
         <f>AVERAGE(B27,B22,B17)</f>
         <v>75.256666666666661</v>
       </c>
@@ -1233,28 +1289,28 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="7">
         <f t="shared" ref="B33:C34" si="0">AVERAGE(B28,B23,B18)</f>
         <v>48.73</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="8">
         <f t="shared" si="0"/>
         <v>14.227316784869977</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="7">
         <f t="shared" si="0"/>
@@ -1265,37 +1321,37 @@
         <v>58.48</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="A39" s="9">
         <f>(SUM(B16:B19)*B7+SUM(C16:C19)*C7+SUM(B21:B24)*B11+SUM(C21:C24)*C11+SUM(B26:B29)*B10+SUM(C26:C29)*C10+SUM(B31:B34)*B3+SUM(C31:C34)*C3)/SUM(B3:C3,B7:C7,B10:C11)</f>
         <v>120.76792682712498</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="A40" s="11">
         <f>A39*About!A27</f>
         <v>154.34141048506572</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1308,13 +1364,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1357,7 +1415,8 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>154.34141048506572</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Remove edits to land use files (may reintroduce in 3.4)
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\AOCoLUPpUA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E0273B-F952-4466-8CA6-022ECA3D5CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,18 +17,7 @@
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -89,6 +72,9 @@
     <t>annual maintenance cost ($ / acre)</t>
   </si>
   <si>
+    <t>Avoid deforestion, peatland restoration, and forest restoration policies</t>
+  </si>
+  <si>
     <t>are not used in the U.S. version of the model.</t>
   </si>
   <si>
@@ -216,15 +202,12 @@
   </si>
   <si>
     <t>timber harvesting need to be managed.</t>
-  </si>
-  <si>
-    <t>Peatland restoration and forest restoration policies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,35 +354,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
+    <cellStyle name="Footnotes: top row" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="5"/>
+    <cellStyle name="Table title" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -409,7 +389,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Conversion Factors"/>
       <sheetName val="About"/>
       <sheetName val="CO2 Aff &amp; Ref"/>
       <sheetName val="VFC-PIIiCRfAaREY"/>
@@ -429,15 +408,10 @@
       <sheetName val="VFC-LVpMCAbAD"/>
       <sheetName val="County Data"/>
       <sheetName val="Forest Mgmt Costs"/>
+      <sheetName val="Conversion Factors"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="A4">
-            <v>3.6666666666666665</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
@@ -456,7 +430,13 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
+      <sheetData sheetId="19">
+        <row r="4">
+          <cell r="A4">
+            <v>3.6666666666666665</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -505,7 +485,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,26 +518,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,23 +553,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,12 +728,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -801,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,17 +755,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>50</v>
+      <c r="B6" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -831,12 +775,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -846,7 +790,7 @@
     </row>
     <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -877,22 +821,22 @@
     <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,27 +844,27 @@
         <v>1.278</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -932,25 +876,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>50+1614</f>
@@ -963,7 +907,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>972+4013</f>
@@ -976,7 +920,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <f>3955+13315</f>
@@ -989,7 +933,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <f>2879+2953</f>
@@ -1002,7 +946,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <f>6236+2826</f>
@@ -1015,7 +959,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <f>2156+2707</f>
@@ -1028,7 +972,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <f>2918+12457</f>
@@ -1041,7 +985,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <f>15095+29814</f>
@@ -1054,7 +998,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <f>10315+29977</f>
@@ -1067,7 +1011,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1075,31 +1019,31 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="8" t="s">
         <v>34</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <f>39/10</f>
@@ -1112,7 +1056,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>95.55</v>
@@ -1121,27 +1065,27 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>44.67</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="10">
         <f>C23*(B18/B23)</f>
         <v>13.041950354609931</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>58.48</v>
@@ -1152,12 +1096,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <f>21.5/10</f>
@@ -1170,7 +1114,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>65.11</v>
@@ -1179,12 +1123,12 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>50.76</v>
@@ -1195,7 +1139,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>58.48</v>
@@ -1206,12 +1150,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <f>21.61/10</f>
@@ -1224,7 +1168,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>65.11</v>
@@ -1233,12 +1177,12 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>50.76</v>
@@ -1249,7 +1193,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>58.48</v>
@@ -1260,12 +1204,12 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <f>24.49/10</f>
@@ -1278,9 +1222,9 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="8">
+        <v>39</v>
+      </c>
+      <c r="B32" s="10">
         <f>AVERAGE(B27,B22,B17)</f>
         <v>75.256666666666661</v>
       </c>
@@ -1289,28 +1233,28 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7">
         <f t="shared" ref="B33:C34" si="0">AVERAGE(B28,B23,B18)</f>
         <v>48.73</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="10">
         <f t="shared" si="0"/>
         <v>14.227316784869977</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="7">
         <f t="shared" si="0"/>
@@ -1321,37 +1265,37 @@
         <v>58.48</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="11">
         <f>(SUM(B16:B19)*B7+SUM(C16:C19)*C7+SUM(B21:B24)*B11+SUM(C21:C24)*C11+SUM(B26:B29)*B10+SUM(C26:C29)*C10+SUM(B31:B34)*B3+SUM(C31:C34)*C3)/SUM(B3:C3,B7:C7,B10:C11)</f>
         <v>120.76792682712498</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="A40" s="13">
         <f>A39*About!A27</f>
         <v>154.34141048506572</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1364,15 +1308,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1415,8 +1357,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <f>'Forest Mgmt Costs'!A40</f>
-        <v>154.34141048506572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>